<commit_message>
add an "is_restricted" field, converted file to text only
</commit_message>
<xml_diff>
--- a/sampledata/qc_events_batch.xlsx
+++ b/sampledata/qc_events_batch.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>facility_id</t>
   </si>
@@ -50,6 +50,18 @@
     <t>file5</t>
   </si>
   <si>
+    <t>is_restricted</t>
+  </si>
+  <si>
+    <t>10083</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>2011-03-17</t>
   </si>
   <si>
@@ -65,6 +77,9 @@
     <t>qc/LCMS_HMSL10083.101.01.pdf</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>2015-03-13</t>
   </si>
   <si>
@@ -74,6 +89,15 @@
     <t>this is the second test</t>
   </si>
   <si>
+    <t>qc/NMR_HMSL10083.101.02.pdf</t>
+  </si>
+  <si>
+    <t>qc/LCMS_HMSL10083.101.02.pdf</t>
+  </si>
+  <si>
+    <t>10001</t>
+  </si>
+  <si>
     <t>2015-11-11</t>
   </si>
   <si>
@@ -86,16 +110,13 @@
     <t>qc/HPLC_HMSL10001.101.01.pdf</t>
   </si>
   <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>2013-01-01</t>
   </si>
   <si>
     <t>all readings were good</t>
+  </si>
+  <si>
+    <t>10002</t>
   </si>
   <si>
     <t>certified by vendor</t>
@@ -183,8 +204,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -213,200 +238,209 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>10083</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>101</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>10083</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>101</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>10001</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>101</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>10001</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>10002</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>101</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>10001</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>101</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>22</v>
+      <c r="F7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add qc events to cell, following small molecule as guide
</commit_message>
<xml_diff>
--- a/sampledata/qc_events_batch.xlsx
+++ b/sampledata/qc_events_batch.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
   <si>
     <t>facility_id</t>
   </si>
@@ -123,6 +123,33 @@
   </si>
   <si>
     <t>second batch passes</t>
+  </si>
+  <si>
+    <t>50001</t>
+  </si>
+  <si>
+    <t>2015-06-03</t>
+  </si>
+  <si>
+    <t>first batch passes</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2015-06-04</t>
+  </si>
+  <si>
+    <t>second batch failed</t>
+  </si>
+  <si>
+    <t>50002</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>bad cell lot</t>
   </si>
 </sst>
 </file>
@@ -133,7 +160,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -159,6 +186,13 @@
       <sz val="10"/>
       <name val="Monospace"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -204,7 +238,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -219,6 +253,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -238,15 +276,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -440,6 +481,98 @@
         <v>29</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>